<commit_message>
Fixes y Avance de administrador
- Fixes pequeños y mejoras de metodos
- Full crud departamentos
- Full crud cursos
- Avances crud estudiantes
</commit_message>
<xml_diff>
--- a/Matriz de trazabilidad.xlsx
+++ b/Matriz de trazabilidad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA 22\Documents\CrisPrince folder\github\SistemaEscuela\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criskop\Documents\GitHub\SistemaEscuelaAlt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C147C3-22D1-43B1-A847-94D16BEA244E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057EA01A-5A9C-4580-ADEE-C92829E24642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="3930" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4245" yWindow="3150" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Información del proyecto" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,24 @@
     <sheet name="Definiciones" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>Información del Proyecto</t>
   </si>
@@ -300,6 +313,21 @@
   </si>
   <si>
     <t>Los usuarios deben tener el campo 'identificacion', con el cual inician sesión</t>
+  </si>
+  <si>
+    <t>horaInicial y horaFinal en la tabla cursos fueron cambiados de DATE a TIME</t>
+  </si>
+  <si>
+    <t>Time es específico para horas</t>
+  </si>
+  <si>
+    <t>fechaInicio y fechaFin en la tabla evaluaciones cambiaron de DATE a DATETIME</t>
+  </si>
+  <si>
+    <t>DATETIME es más preciso para el día y hora</t>
+  </si>
+  <si>
+    <t>fechaEntrega en la tabla calificaciones fue cambiado de DATE a DATETIME</t>
   </si>
 </sst>
 </file>
@@ -956,7 +984,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1028,7 +1056,7 @@
       </c>
       <c r="D6" s="14">
         <f ca="1">TODAY()</f>
-        <v>45786</v>
+        <v>45795</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>41</v>
@@ -1056,7 +1084,7 @@
       </c>
       <c r="D7" s="14">
         <f ca="1">TODAY()</f>
-        <v>45786</v>
+        <v>45795</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>41</v>
@@ -1076,36 +1104,87 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="14">
+        <f ca="1">TODAY()</f>
+        <v>45795</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="14">
+        <f ca="1">TODAY()</f>
+        <v>45795</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="14">
+        <f ca="1">TODAY()</f>
+        <v>45795</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>

</xml_diff>